<commit_message>
finish main data cleaning and create outline of shiny app
</commit_message>
<xml_diff>
--- a/2-shiny-app/data/keywords.xlsx
+++ b/2-shiny-app/data/keywords.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="49">
   <si>
     <t>Age</t>
   </si>
@@ -267,6 +267,18 @@
   </si>
   <si>
     <t>year</t>
+  </si>
+  <si>
+    <t>XX</t>
+  </si>
+  <si>
+    <t>Do you currently have a mental health disorder?</t>
+  </si>
+  <si>
+    <t>cuurently.have.</t>
+  </si>
+  <si>
+    <t>interpolate [[1]]</t>
   </si>
 </sst>
 </file>
@@ -325,7 +337,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -342,6 +354,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -648,10 +663,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D28"/>
+  <dimension ref="A1:D29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -659,6 +674,7 @@
     <col min="1" max="1" width="6.5546875" customWidth="1"/>
     <col min="2" max="2" width="61" style="3" customWidth="1"/>
     <col min="3" max="3" width="52.77734375" style="3" customWidth="1"/>
+    <col min="4" max="4" width="21.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
@@ -748,209 +764,223 @@
       <c r="D7" s="5"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" s="4">
-        <v>8</v>
+      <c r="A8" s="4" t="s">
+        <v>45</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="D8" s="5"/>
+        <v>46</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="4">
+        <v>8</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D9" s="5"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="4">
         <v>9</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B10" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C10" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="D9" s="5"/>
-    </row>
-    <row r="10" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A10" s="4">
+      <c r="D10" s="5"/>
+    </row>
+    <row r="11" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A11" s="4">
         <v>10</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B11" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C11" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D11" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" s="4">
-        <v>11</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="D11" s="5"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="4">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C12" s="7"/>
+        <v>8</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>32</v>
+      </c>
       <c r="D12" s="5"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="4">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>34</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="C13" s="7"/>
       <c r="D13" s="5"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="4">
+        <v>13</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D14" s="5"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" s="4">
         <v>14</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B15" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C15" s="3" t="s">
         <v>35</v>
-      </c>
-      <c r="D14" s="5"/>
-    </row>
-    <row r="15" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A15" s="4">
-        <v>15</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>36</v>
       </c>
       <c r="D15" s="5"/>
     </row>
     <row r="16" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A16" s="4">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>13</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D16" s="5"/>
     </row>
     <row r="17" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A17" s="4">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A18" s="4">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A19" s="4">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A20" s="4">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>37</v>
+        <v>16</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A21" s="4">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A22" s="4">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A23" s="4">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A24" s="4">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A25" s="4">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A26" s="4">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>17</v>
+        <v>42</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A27" s="4">
+        <v>26</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A28" s="4">
         <v>27</v>
       </c>
-      <c r="B27" s="3" t="s">
+      <c r="B28" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A28" s="4">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A29" s="4">
         <v>28</v>
       </c>
-      <c r="B28" s="3" t="s">
+      <c r="B29" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C28" s="7"/>
-      <c r="D28" s="5"/>
+      <c r="C29" s="7"/>
+      <c r="D29" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>